<commit_message>
Added comments to the following classes: DataAccessor and AirQualitySensor. Added a theme/fonts to the powerpoint and content to the road map slide
</commit_message>
<xml_diff>
--- a/ExcelFiles/TRAD-IT-Timesheet.xlsx
+++ b/ExcelFiles/TRAD-IT-Timesheet.xlsx
@@ -56,20 +56,19 @@
     <t>Hours Worked</t>
   </si>
   <si>
-    <t>1:15pm</t>
-  </si>
-  <si>
-    <t>Started going through the codebase and adding comments to make the code more readable and understandable. Added comments to the follwing classes: EmailHandler, DataAcessor. Restructured the folders in the visual studio solution. Was working in the wrong branch of git so I had to go back and re add them.  Created a timesheet to track hours worked.</t>
+    <t>Started going through the codebase and adding comments to make the code more readable and understandable. Added comments to the follwing classes: EmailHandler, DataAcessor, AirQualitySensor. Restructured the folders in the visual studio solution. Was working in the wrong branch of git so I had to go back and re add them.  Created a timesheet to track hours worked. Still need to finish the AQS comments. Worked on the presentation by adding a theme, changing the fonts, and adding content to the road map</t>
+  </si>
+  <si>
+    <t>2:30pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -209,10 +208,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,7 +540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -552,13 +551,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="13">
+        <v>4.75</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="13">
-        <v>3.5</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>